<commit_message>
Added Charts on admin and office capabiliteis VIA PHPoffice improved
</commit_message>
<xml_diff>
--- a/public/report.xlsx
+++ b/public/report.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
   <si>
     <t># of Users</t>
   </si>
@@ -30,6 +30,15 @@
   </si>
   <si>
     <t>Students</t>
+  </si>
+  <si>
+    <t>Total Actv.</t>
+  </si>
+  <si>
+    <t>No. of Scores</t>
+  </si>
+  <si>
+    <t>Total Statistics</t>
   </si>
 </sst>
 </file>
@@ -365,7 +374,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -373,12 +382,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -392,7 +401,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>7</v>
       </c>
@@ -403,6 +412,87 @@
         <v>4</v>
       </c>
       <c r="D4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10">
+        <v>0</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>4</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13"/>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17" t="s">
+        <v>2</v>
+      </c>
+      <c r="E17" t="s">
+        <v>3</v>
+      </c>
+      <c r="F17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18">
+        <v>0</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>7</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>4</v>
+      </c>
+      <c r="F18">
         <v>2</v>
       </c>
     </row>
@@ -410,6 +500,8 @@
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <mergeCells>
     <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A13:F13"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Teacher added with student manipulation and ide
</commit_message>
<xml_diff>
--- a/public/report.xlsx
+++ b/public/report.xlsx
@@ -403,10 +403,10 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C4">
         <v>4</v>
@@ -484,10 +484,10 @@
         <v>0</v>
       </c>
       <c r="C18">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E18">
         <v>4</v>

</xml_diff>

<commit_message>
add auto saveblock capabilities
</commit_message>
<xml_diff>
--- a/public/report.xlsx
+++ b/public/report.xlsx
@@ -403,7 +403,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -412,7 +412,7 @@
         <v>4</v>
       </c>
       <c r="D4">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -436,16 +436,16 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C10">
         <v>4</v>
       </c>
       <c r="D10">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -478,13 +478,13 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C18">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D18">
         <v>2</v>
@@ -493,7 +493,7 @@
         <v>4</v>
       </c>
       <c r="F18">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Code Generator as a  Python code and display it on a codemirror.js editor in readonly
</commit_message>
<xml_diff>
--- a/public/report.xlsx
+++ b/public/report.xlsx
@@ -403,13 +403,13 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4">
         <v>2</v>
       </c>
       <c r="C4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D4">
         <v>4</v>
@@ -436,13 +436,13 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C10">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D10">
         <v>4</v>
@@ -478,19 +478,19 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C18">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D18">
         <v>2</v>
       </c>
       <c r="E18">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F18">
         <v>4</v>

</xml_diff>